<commit_message>
Lobby and Stage Scene
</commit_message>
<xml_diff>
--- a/Unity/DataTable.xlsx
+++ b/Unity/DataTable.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
@@ -1659,63 +1659,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Images/Button/BookStage_Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StageBarSelectBtn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images/Button/BookStage_Select</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CloseDownBtn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images/Button/CloseButton_Down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CloseNormalBtn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images/Button/CloseButton_Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoDownBtn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images/Button/IngameGo_Down</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GoNormalBtn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images/Button/IngameGo_Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thief</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Images/Character/021_P_YL_Theif_Nor_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Thief</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>StageBarNormalBtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Button/BookStage_Normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>StageBarSelectBtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Button/BookStage_Select</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CloseDownBtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Button/CloseButton_Down</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CloseNormalBtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Button/CloseButton_Normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GoDownBtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Button/IngameGo_Down</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>GoNormalBtn</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Button/IngameGo_Normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thief</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Images/Character/021_P_YL_Theif_Nor_001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Thief</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2584,7 +2584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A112" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
@@ -4261,7 +4261,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="58" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E60" s="58" t="s">
         <v>72</v>
@@ -7514,7 +7514,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G90" sqref="G90"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9252,8 +9252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -9378,10 +9378,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>415</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -9521,10 +9521,10 @@
         <v>205</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>403</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -9532,10 +9532,10 @@
         <v>206</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>405</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -9543,10 +9543,10 @@
         <v>207</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>407</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -9554,10 +9554,10 @@
         <v>208</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>409</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>410</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -9565,10 +9565,10 @@
         <v>209</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>411</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -9576,10 +9576,10 @@
         <v>210</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>414</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add MonsterTable and PlayerLevelTable
</commit_message>
<xml_diff>
--- a/Unity/DataTable.xlsx
+++ b/Unity/DataTable.xlsx
@@ -9,12 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Dialog" sheetId="1" r:id="rId1"/>
     <sheet name="Scenario" sheetId="2" r:id="rId2"/>
     <sheet name="ImageData" sheetId="3" r:id="rId3"/>
+    <sheet name="MonsterTable" sheetId="4" r:id="rId4"/>
+    <sheet name="PlayerLevelTable" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -180,7 +182,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="713" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="740" uniqueCount="443">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1716,6 +1718,93 @@
   </si>
   <si>
     <t>BackNormalBtn</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>S_Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R_Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>P_Rate</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ActivateEpi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GameCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mon1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mon2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mon3</t>
+  </si>
+  <si>
+    <t>Mon4</t>
+  </si>
+  <si>
+    <t>Mon5</t>
+  </si>
+  <si>
+    <t>Mon6</t>
+  </si>
+  <si>
+    <t>Mon7</t>
+  </si>
+  <si>
+    <t>Mon8</t>
+  </si>
+  <si>
+    <t>Mon9</t>
+  </si>
+  <si>
+    <t>Mon10</t>
+  </si>
+  <si>
+    <t>Mon11</t>
+  </si>
+  <si>
+    <t>Mon12</t>
+  </si>
+  <si>
+    <t>Mon13</t>
+  </si>
+  <si>
+    <t>Mon14</t>
+  </si>
+  <si>
+    <t>Mon15</t>
+  </si>
+  <si>
+    <t>InactivateEpi</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Level</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LoseCount</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LevelUpCount</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1769,7 +1858,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1833,6 +1922,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2018,7 +2113,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2299,6 +2394,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2584,7 +2685,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
@@ -9587,4 +9688,758 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="5" width="9" style="1"/>
+    <col min="6" max="6" width="12.125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14" style="1" customWidth="1"/>
+    <col min="8" max="8" width="14.625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="95" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="94" t="s">
+        <v>418</v>
+      </c>
+      <c r="C1" s="94" t="s">
+        <v>420</v>
+      </c>
+      <c r="D1" s="94" t="s">
+        <v>419</v>
+      </c>
+      <c r="E1" s="94" t="s">
+        <v>421</v>
+      </c>
+      <c r="F1" s="94" t="s">
+        <v>422</v>
+      </c>
+      <c r="G1" s="94" t="s">
+        <v>439</v>
+      </c>
+      <c r="H1" s="94" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="C2" s="1">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1">
+        <v>20</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2</v>
+      </c>
+      <c r="H2" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="C3" s="1">
+        <v>40</v>
+      </c>
+      <c r="D3" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>3</v>
+      </c>
+      <c r="H3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="D4" s="1">
+        <v>40</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1">
+        <v>5</v>
+      </c>
+      <c r="H4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="C5" s="1">
+        <v>10</v>
+      </c>
+      <c r="D5" s="1">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40</v>
+      </c>
+      <c r="F5" s="1">
+        <v>2</v>
+      </c>
+      <c r="G5" s="1">
+        <v>7</v>
+      </c>
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="C6" s="1">
+        <v>60</v>
+      </c>
+      <c r="D6" s="1">
+        <v>20</v>
+      </c>
+      <c r="E6" s="1">
+        <v>20</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1">
+        <v>6</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="C7" s="1">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>90</v>
+      </c>
+      <c r="F7" s="1">
+        <v>4</v>
+      </c>
+      <c r="G7" s="1">
+        <v>8</v>
+      </c>
+      <c r="H7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C8" s="1">
+        <v>30</v>
+      </c>
+      <c r="D8" s="1">
+        <v>30</v>
+      </c>
+      <c r="E8" s="1">
+        <v>40</v>
+      </c>
+      <c r="F8" s="1">
+        <v>4</v>
+      </c>
+      <c r="G8" s="1">
+        <v>9</v>
+      </c>
+      <c r="H8" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C9" s="1">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <v>70</v>
+      </c>
+      <c r="E9" s="1">
+        <v>5</v>
+      </c>
+      <c r="F9" s="1">
+        <v>5</v>
+      </c>
+      <c r="G9" s="1">
+        <v>6</v>
+      </c>
+      <c r="H9" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C10" s="1">
+        <v>25</v>
+      </c>
+      <c r="D10" s="1">
+        <v>50</v>
+      </c>
+      <c r="E10" s="1">
+        <v>25</v>
+      </c>
+      <c r="F10" s="1">
+        <v>5</v>
+      </c>
+      <c r="G10" s="1">
+        <v>7</v>
+      </c>
+      <c r="H10" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C11" s="1">
+        <v>80</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+      <c r="E11" s="1">
+        <v>15</v>
+      </c>
+      <c r="F11" s="1">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1">
+        <v>9</v>
+      </c>
+      <c r="H11" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C12" s="1">
+        <v>25</v>
+      </c>
+      <c r="D12" s="1">
+        <v>55</v>
+      </c>
+      <c r="E12" s="1">
+        <v>20</v>
+      </c>
+      <c r="F12" s="1">
+        <v>6</v>
+      </c>
+      <c r="G12" s="1">
+        <v>10</v>
+      </c>
+      <c r="H12" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C13" s="1">
+        <v>50</v>
+      </c>
+      <c r="D13" s="1">
+        <v>10</v>
+      </c>
+      <c r="E13" s="1">
+        <v>40</v>
+      </c>
+      <c r="F13" s="1">
+        <v>7</v>
+      </c>
+      <c r="G13" s="1">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C14" s="1">
+        <v>10</v>
+      </c>
+      <c r="D14" s="1">
+        <v>80</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10</v>
+      </c>
+      <c r="F14" s="1">
+        <v>7</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15</v>
+      </c>
+      <c r="D15" s="1">
+        <v>15</v>
+      </c>
+      <c r="E15" s="1">
+        <v>70</v>
+      </c>
+      <c r="F15" s="1">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1">
+        <v>10</v>
+      </c>
+      <c r="H15" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C16" s="1">
+        <v>25</v>
+      </c>
+      <c r="D16" s="1">
+        <v>35</v>
+      </c>
+      <c r="E16" s="1">
+        <v>40</v>
+      </c>
+      <c r="F16" s="1">
+        <v>9</v>
+      </c>
+      <c r="G16" s="1">
+        <v>10</v>
+      </c>
+      <c r="H16" s="1">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="2" width="9" style="1"/>
+    <col min="3" max="3" width="12.125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.625" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="95" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="94" t="s">
+        <v>440</v>
+      </c>
+      <c r="C1" s="94" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="94" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5</v>
+      </c>
+      <c r="C6" s="1">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6</v>
+      </c>
+      <c r="C7" s="1">
+        <v>3</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9</v>
+      </c>
+      <c r="C10" s="1">
+        <v>4</v>
+      </c>
+      <c r="D10" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10</v>
+      </c>
+      <c r="C11" s="1">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1">
+        <v>5</v>
+      </c>
+      <c r="D12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1">
+        <v>5</v>
+      </c>
+      <c r="D13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13</v>
+      </c>
+      <c r="C14" s="1">
+        <v>5</v>
+      </c>
+      <c r="D14" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14</v>
+      </c>
+      <c r="C15" s="1">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6</v>
+      </c>
+      <c r="D16" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6</v>
+      </c>
+      <c r="D17" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17</v>
+      </c>
+      <c r="C18" s="1">
+        <v>6</v>
+      </c>
+      <c r="D18" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18</v>
+      </c>
+      <c r="C19" s="1">
+        <v>6</v>
+      </c>
+      <c r="D19" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19</v>
+      </c>
+      <c r="C20" s="1">
+        <v>7</v>
+      </c>
+      <c r="D20" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20</v>
+      </c>
+      <c r="C21" s="1">
+        <v>7</v>
+      </c>
+      <c r="D21" s="1">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Finish minigame and Add EffectManager
</commit_message>
<xml_diff>
--- a/Unity/DataTable.xlsx
+++ b/Unity/DataTable.xlsx
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="753" uniqueCount="455">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="461">
   <si>
     <t>Index</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1854,6 +1854,30 @@
   </si>
   <si>
     <t>Prefabs/UI/MiniGameUI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MouseClick</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Effects/CFX_Explosion_B_Smoke+Text</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MiniGameWin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Effects/CFX2_PickupSmiley2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MiniGameLose</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Prefabs/Effects/CFX_Hit_A Red+RandomText</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -10495,17 +10519,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="9" style="1"/>
-    <col min="2" max="2" width="14.625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="23" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45.125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -10572,6 +10596,39 @@
       </c>
       <c r="C6" s="1" t="s">
         <v>454</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>460</v>
       </c>
     </row>
   </sheetData>

</xml_diff>